<commit_message>
ready to submit, updated README
</commit_message>
<xml_diff>
--- a/task1_data.xlsx
+++ b/task1_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonic\Documents\CMSC\CMSC-312\CMSC312_OS_As3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42144D87-3E56-4FD3-8ECA-E97F6D5097FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087D2020-208C-43DA-81D0-58B5D34CB105}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A7CD66A2-B7C2-4254-802D-CA7398CB00D7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A7CD66A2-B7C2-4254-802D-CA7398CB00D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
   <si>
     <t>Producers</t>
   </si>
@@ -52,6 +52,24 @@
   </si>
   <si>
     <t>Producers = 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consumers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LIFO </t>
+  </si>
+  <si>
+    <t>SJF</t>
+  </si>
+  <si>
+    <t>LIFO</t>
+  </si>
+  <si>
+    <t>Producers = 4</t>
+  </si>
+  <si>
+    <t>Producers = 6</t>
   </si>
 </sst>
 </file>
@@ -156,9 +174,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -493,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9785B5AE-D2FF-4AD4-84FB-E8F2A2910F95}">
-  <dimension ref="A2:E22"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,314 +527,638 @@
     <col min="2" max="5" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="E4" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D5" s="2">
         <v>4.8999999999999998E-5</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E5" s="2">
         <v>9.9852319999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C6" s="2">
         <v>5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D6" s="2">
         <v>1.7699999999999999E-4</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E6" s="2">
         <v>1.7979259999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B7" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C7" s="2">
         <v>10</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D7" s="2">
         <v>9.2E-5</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E7" s="2">
         <v>8.2267309999999991</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C8" s="2">
         <v>5</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D8" s="2">
         <v>3.6200000000000002E-4</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E8" s="2">
         <v>11.47823</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1">
-        <v>10</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1.03E-4</v>
-      </c>
-      <c r="E7" s="1">
-        <v>13.144556</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1.56E-4</v>
-      </c>
-      <c r="E8" s="1">
-        <v>10.523792</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.03E-4</v>
+      </c>
+      <c r="E9" s="2">
+        <v>13.144556</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.56E-4</v>
+      </c>
+      <c r="E10" s="2">
+        <v>10.523792</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B11" s="2">
         <v>100</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C11" s="2">
         <v>100</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D11" s="2">
         <v>2.7070000000000002E-3</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E11" s="2">
         <v>17.698281000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B12" s="2">
         <v>50</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C12" s="2">
         <v>100</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D12" s="2">
         <v>1.6200000000000001E-4</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E12" s="2">
         <v>15.574923999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B13" s="2">
         <v>25</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C13" s="2">
         <v>100</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D13" s="2">
         <v>2.14E-4</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E13" s="2">
         <v>15.116909</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B14" s="2">
         <v>15</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C14" s="2">
         <v>1</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D14" s="2">
         <v>14.507783999999999</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E14" s="2">
         <v>65.108749000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B15" s="2">
         <v>15</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C15" s="2">
         <v>10</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D15" s="2">
         <v>0.56332899999999997</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E15" s="2">
         <v>12.640392</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B16" s="2">
         <v>15</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C16" s="2">
         <v>15</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D16" s="2">
         <v>1.7699999999999999E-4</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E16" s="2">
         <v>13.385755</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B17" s="2">
         <v>1000</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C17" s="2">
         <v>1000</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D17" s="2">
         <v>0.29387000000000002</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E17" s="2">
         <v>30.598410999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B18" s="2">
         <v>100</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C18" s="2">
         <v>1000</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D18" s="2">
         <v>8.3160000000000005E-3</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E18" s="2">
         <v>16.544259</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="6">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
         <v>15</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B19" s="2">
         <v>10</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C19" s="2">
         <v>1000</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D19" s="2">
         <v>9.5200000000000005E-4</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E19" s="2">
         <v>11.585944</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>2</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>4</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>6</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>8</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>10</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>2</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>4</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>6</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>8</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>10</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>2</v>
+      </c>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>4</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>6</v>
+      </c>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>8</v>
+      </c>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>10</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>2</v>
+      </c>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>4</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>6</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>8</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>10</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
+        <v>2</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <v>4</v>
+      </c>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <v>6</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <v>8</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <v>10</v>
+      </c>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>